<commit_message>
all kinds of updates
</commit_message>
<xml_diff>
--- a/data/all_exclude_country_lists_isin.xlsx
+++ b/data/all_exclude_country_lists_isin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anja\OneDrive - Gravercentret\Dokumenter\Python_projekter\kommune_investering\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F140F4-2CA4-44FA-8BC3-088DF153DAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C221DA1E-1391-49C8-8F00-AEE186C37698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="310">
   <si>
     <t>ISIN</t>
   </si>
@@ -947,6 +947,9 @@
   </si>
   <si>
     <t>Menneskerettigheder; Emerging Markets statsobligationer, som ikke lever op til ESG-kriterier; Ekskluderer lande, som enten er underlagt internationale sanktioner, eller som PFA har vurderet som ikke-investeringsegnede.</t>
+  </si>
+  <si>
+    <t>XS2294323386</t>
   </si>
 </sst>
 </file>
@@ -1314,18 +1317,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H154"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1351,7 +1354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1455,7 +1458,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -2131,7 +2134,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -2287,7 +2290,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -2313,7 +2316,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2443,7 +2446,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2521,7 +2524,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2547,7 +2550,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2573,7 +2576,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2625,7 +2628,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2651,7 +2654,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2703,7 +2706,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2755,7 +2758,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2833,7 +2836,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2859,7 +2862,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2911,7 +2914,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -2963,7 +2966,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2989,7 +2992,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -3015,7 +3018,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -3067,7 +3070,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -3093,7 +3096,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -3119,7 +3122,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -3171,7 +3174,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -3223,7 +3226,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -3249,7 +3252,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -3275,7 +3278,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -3301,7 +3304,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -3353,7 +3356,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -3379,7 +3382,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -3431,7 +3434,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -3483,7 +3486,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -3535,7 +3538,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -3561,7 +3564,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -3587,7 +3590,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -3613,7 +3616,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3639,7 +3642,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -3665,7 +3668,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -3691,7 +3694,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -3743,7 +3746,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -3769,7 +3772,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -3795,7 +3798,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -3821,7 +3824,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -3847,7 +3850,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -3873,7 +3876,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -3899,7 +3902,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -3951,7 +3954,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -4003,7 +4006,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -4029,7 +4032,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -4055,7 +4058,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -4081,7 +4084,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -4107,7 +4110,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -4133,7 +4136,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -4159,7 +4162,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -4185,7 +4188,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -4211,7 +4214,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -4237,7 +4240,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -4263,7 +4266,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -4289,7 +4292,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -4315,7 +4318,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -4341,7 +4344,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -4367,7 +4370,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -4393,7 +4396,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -4419,7 +4422,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -4445,7 +4448,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -4471,7 +4474,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -4497,7 +4500,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -4523,7 +4526,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -4549,7 +4552,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -4575,7 +4578,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -4601,7 +4604,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -4627,7 +4630,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -4653,7 +4656,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -4679,7 +4682,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>136</v>
       </c>
@@ -4705,7 +4708,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -4731,7 +4734,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -4757,7 +4760,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -4783,7 +4786,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -4809,7 +4812,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>141</v>
       </c>
@@ -4835,7 +4838,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>142</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -4887,7 +4890,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -4913,7 +4916,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -4939,7 +4942,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>146</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -4991,7 +4994,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>148</v>
       </c>
@@ -5017,7 +5020,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -5043,7 +5046,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>150</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -5095,7 +5098,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>152</v>
       </c>
@@ -5121,7 +5124,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>153</v>
       </c>
@@ -5147,7 +5150,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>155</v>
       </c>
@@ -5199,7 +5202,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>156</v>
       </c>
@@ -5225,7 +5228,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>158</v>
       </c>
@@ -5277,7 +5280,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>159</v>
       </c>
@@ -5303,7 +5306,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>160</v>
       </c>
@@ -5327,6 +5330,32 @@
       </c>
       <c r="H154" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>309</v>
+      </c>
+      <c r="B155" t="s">
+        <v>180</v>
+      </c>
+      <c r="C155" t="s">
+        <v>198</v>
+      </c>
+      <c r="D155" t="s">
+        <v>214</v>
+      </c>
+      <c r="E155" t="s">
+        <v>236</v>
+      </c>
+      <c r="F155" t="s">
+        <v>263</v>
+      </c>
+      <c r="G155" t="s">
+        <v>288</v>
+      </c>
+      <c r="H155" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>